<commit_message>
update test case of entitymgmt
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-entity-management-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E910C88C-0219-40C1-ACB6-EAAA4A6FE971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6796B4C5-1587-4544-82AC-96F566DB29A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publishCheck" sheetId="21" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="393">
   <si>
     <t>testEntity1</t>
   </si>
@@ -3854,6 +3854,22 @@
   <si>
     <t>snc-entityMgmt-publishCheck-update-Test-22</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity [[abcde123]] not exist</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Validation failed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOT_EXIST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Edge [[abcde123]] not exist</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5612,8 +5628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F5FE0E-8788-403D-8502-6CD26A71119B}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5740,12 +5756,12 @@
         <v>86</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>89</v>
+        <v>390</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6" t="s">
-        <v>140</v>
+        <v>391</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -5767,11 +5783,13 @@
         <v>86</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>141</v>
+        <v>390</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="K5" s="6" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
@@ -5814,7 +5832,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5889,7 +5907,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>72</v>
       </c>
@@ -5909,7 +5927,7 @@
         <v>101400</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>141</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
@@ -6230,7 +6248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F350B3-2BA8-4FFC-BD4B-B88814906262}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -7371,12 +7389,12 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.5546875" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.6640625" style="5" bestFit="1" customWidth="1"/>
@@ -7489,12 +7507,12 @@
         <v>86</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>89</v>
+        <v>390</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>140</v>
+        <v>391</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -7515,11 +7533,13 @@
         <v>86</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>141</v>
+        <v>390</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="J5" s="6" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
@@ -7561,7 +7581,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E8" sqref="E8:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7629,7 +7649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>39</v>
       </c>
@@ -7648,7 +7668,7 @@
         <v>101400</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>141</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>